<commit_message>
Pre frontend Working Backend
</commit_message>
<xml_diff>
--- a/scrapy/static/data/Lodha+bhandup+Ad+Advertiser.xlsx
+++ b/scrapy/static/data/Lodha+bhandup+Ad+Advertiser.xlsx
@@ -454,16 +454,17 @@
       <c r="A2" t="inlineStr">
         <is>
           <t>Sponsored
-Lodha Bhandup New Project - 2&amp;3BHK Starts ₹ 2.29 Cr All in
-newproject-bhandup.co.in
-https://www.newproject-bhandup.co.in › lodha › new-launch
-Lodha New Launch Luxurious 2 &amp; 3 BHK apartments Starting Price from ₹ 2.29 Cr All Inc
-Price List · Brochure · Configuration · Request Site Visit</t>
+Lödha Bhandup | Luxury 2, 2.5 &amp; 3 BHK - Avail Pre Launch Offer
+l-bhandup.com
+https://www.l-bhandup.com › official
+Lödha on LBS Rd an upcoming residential project with the best of amenities &amp; views. Pre Launch Offer. EOI Bookings Open, Pay just...
+Brochure &amp; Floor Plans · Price · Connect on Whatsapp · View Project Highlights
+Deal: Up to ₹500,000 off Pre Launch Offer</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>AddressofChoice Realty Pvt. Ltd</t>
+          <t>Rioga Premium Real Estate Advisory LLP</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -476,16 +477,16 @@
       <c r="A3" t="inlineStr">
         <is>
           <t>Sponsored
-Lödha Bhandup West - Luxury 2, 2.5 &amp; 3 BHK
-l-bhandup.com
-https://www.l-bhandup.com › official
-Lödha on LBS Rd an upcoming residential project with the best of amenities ...
-Deal: Up to ₹500,000 off Pre Launch Offer</t>
+Lodha Bhandup - New Project Launch in Bhandup
+proptigermumbai.com
+https://www.proptigermumbai.com
+its Big Apartments with 2/3 BHK, its prime Location along the LBS Road, Starts @ ₹ 2.29Cr* The Apartments have 2/3 BHK Configurations &amp; are Designed to Provide Ample Space &amp; Comfort. New Launch Project. Easy Payment Plan. Flexible Payment Plan. Budget Friendly.
+Pricing &amp; Floor Plan · Download Brochure · Runwal Group · Platinum Group · Adani Realty</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Rioga Premium Real Estate Advisory LLP</t>
+          <t>Locon Solutions Pvt. Ltd.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -498,16 +499,16 @@
       <c r="A4" t="inlineStr">
         <is>
           <t>Sponsored
-Bhandup, Mumbai - 2/3 BHK from 2.29 Cr*
-new-launch-project.in
-https://www.new-launch-project.in
-Price starts from 2.29 Cr* onwards. Call for more details. Download Brochure. New Launch...
-Pricing · Site and Floorplan · Amenities · Sitevisit</t>
+New Launch At Bhandup, Mumbai | New Launch At Bhandup
+lódháhomz.site
+https://www.lódháhomz.site › visit-site › enquire-now
+New Launch At Bhandup provides ultra-luxurious residences with the most breathtaking views
+E-Brochure · Pricing / Costing · Floor Plan · Project Overview</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Elegance Enterprises</t>
+          <t>DIGITAL RUBIX</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -520,20 +521,20 @@
       <c r="A5" t="inlineStr">
         <is>
           <t>Sponsored
-Lodha Bhandup West Mumbai - 2&amp;3 BHK Apartment @ ₹2.29 CR*
-india-sales-office.com
-https://www.india-sales-office.com
-Starts at ₹2.29 CR* | The prime LBS Road, Mumbai | Modern Homes | Lots of Space &amp; Comfort.</t>
+Lodha Prelaunching Bhandup - 2 &amp; 3 BHK Starting ₹2.29 Cr*
+prelaunch-projects.in
+https://www.prelaunch-projects.in › lodhabhandup › luxuryhomes
+Get EOI and Early Bird Benefits, Prime location at LBS Road Bhandup by Lodha. Lodha...</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Property Junction International Real Estate Broker LLC</t>
+          <t>PRELAUNCH REALTY PRIVATE LIMITED</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>United Arab Emirates</t>
+          <t>India</t>
         </is>
       </c>
     </row>
@@ -541,16 +542,15 @@
       <c r="A6" t="inlineStr">
         <is>
           <t>Sponsored
-New Launch @ Bhandup by Lodha | 2 &amp; 3 BHK Starting ₹2.29 Cr*
-prelaunch-projects.in
-https://www.prelaunch-projects.in › lodhabhandup › luxuryhomes
-Get EOI and Early Bird Benefits, Prime location at LBS Road Bhandup by Lodha. Lodha Bhandup 2 &amp; 3 BHK Homes Starting Price...
-Price Plans · Project Location · Site &amp; Floor Plan · The Amenities · Virtual Site Visit</t>
+Lodha New Launch Bhandup | Luxury 2 &amp; 3 BHK
+bhandupnewlaunch.com
+https://www.bhandupnewlaunch.com › 2&amp;3bhk › luxury_homes
+Pre-book Lodha Bhandup at ₹1.08 Lacs* | Easy Access to Powai &amp; R-City Mall | EOI Open Now! Modern Living at Lodha Bhandup | 10 mins to Eastern Express Hwy | Pre-book at ₹1.08 Lacs* Free Pickup &amp; Drop. Avail Special Offers. Book Now.</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>PRELAUNCH REALTY PRIVATE LIMITED</t>
+          <t>Finwizz Holdings</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -563,16 +563,15 @@
       <c r="A7" t="inlineStr">
         <is>
           <t>Sponsored
-New Launch Lodha Bhandup | 2 &amp; 3 BHK Homes at ₹ 2.29 Cr*
-newlaunch-bhandup.co.in
-https://www.newlaunch-bhandup.co.in › new_launch
-Luxury 2 &amp; 3 BHK Homes Starts From ₹ 2.29 Cr* All Incl at Lodha Bhandup West, Mumbai. The project has easy access to both the Eastern Express Highway and the Eastern Motorway. Exclusive Offer. Get The Best Rate.
-Pricing · View Gallery · Site &amp; Floor Plans · Our Location · Proposed Floor Plan · Location</t>
+Lodha® LBS is Coming Soon
+lodhagroup.in
+https://www.lodhagroup.in
+Lodha® coming soon to LBS — Live an exceptional lifestyle with forest living as Lodha comes to the prime LBS Marg. Lodha LBS along the Mulund-Bhandup-Kanjurmarg corridor ensures seamless connectivity.</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Propertypistol Realty Pvt ltd</t>
+          <t>Macrotech Developers Limited</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -585,16 +584,16 @@
       <c r="A8" t="inlineStr">
         <is>
           <t>Sponsored
-Lodha Bhandup West | 2, 2.5 &amp; 3 BHK Residences
-luxurypropertiesbhandup.com
-https://www.luxurypropertiesbhandup.com › new_launch › enquire_now
-Lodha Bhandup Luxury 2 &amp; 3 BHK Homes Starts From ₹ 2.29 Cr* All Incl at Bhandup, Mumbai. Living. Lodha Is Launching Luxurious 2, 2.5 &amp; 3 BHK Residences at a Very...
-Pricing Details · Project Plans · Project Amenities · Project Overview</t>
+Lodha Bhandup | Lodha Bhandup New Launch
+propertymumbai.co.in
+http://www.propertymumbai.co.in › lodha_bhandup
+Book 2 &amp; 3 BHK Starts ₹2.29 Cr* &amp; Get EOI &amp; Early Bird Benefits at New Launch Bhandup West. its Big Apartments with 2/3 BHK, its prime Location along the LBS Road, Starts @ ₹ 2.29Cr* Download Brochure.
+Price · Floor Plan · Location · Amenities</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>NYNEX Realty Venture Pvt. Ltd.</t>
+          <t>NORA GROUP</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">

</xml_diff>

<commit_message>
UI for dashboard, changes in Index
</commit_message>
<xml_diff>
--- a/scrapy/static/data/Lodha+bhandup+Ad+Advertiser.xlsx
+++ b/scrapy/static/data/Lodha+bhandup+Ad+Advertiser.xlsx
@@ -454,61 +454,60 @@
       <c r="A2" t="inlineStr">
         <is>
           <t>Sponsored
-Lödha Bhandup | Luxury 2, 2.5 &amp; 3 BHK - Avail Pre Launch Offer
+Lodha Bhandup New Project - 2 &amp; 3 BHK @ ₹ 2.29 Cr All inc
+newproject-bhandup.co.in
+https://www.newproject-bhandup.co.in › lodha › new-launch
+Lodha New Launch Luxurious 2 &amp; 3 BHK apartments Starting Price from ₹ 2.29 Cr All Inc
+Price List · Brochure · Request Site Visit · Configuration</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>AddressofChoice Realty Pvt. Ltd</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Sponsored
+Lodha Bhandup | New Project Launch in Bhandup
+proptigermumbai.com
+https://www.proptigermumbai.com
+New Launch Project — its Big Apartments with 2/3 BHK, its prime Location along the LBS...
+Pricing &amp; Floor Plan · Download Brochure · Runwal Group · Platinum Group · Adani Realty</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Locon Solutions Pvt. Ltd.</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Sponsored
+Lödha Bhandup | Luxury 2, 2.5 &amp; 3 BHK | Avail Pre Launch Offer
 l-bhandup.com
 https://www.l-bhandup.com › official
-Lödha on LBS Rd an upcoming residential project with the best of amenities &amp; views. Pre Launch Offer. EOI Bookings Open, Pay just...
-Brochure &amp; Floor Plans · Price · Connect on Whatsapp · View Project Highlights
-Deal: Up to ₹500,000 off Pre Launch Offer</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
+Excellent Connectivity — Lödha on LBS Rd an upcoming residential project with the best of...
+Brochure &amp; Floor Plans · Connect on Whatsapp · Price · View Project Highlights</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>Rioga Premium Real Estate Advisory LLP</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Sponsored
-Lodha Bhandup - New Project Launch in Bhandup
-proptigermumbai.com
-https://www.proptigermumbai.com
-its Big Apartments with 2/3 BHK, its prime Location along the LBS Road, Starts @ ₹ 2.29Cr* The Apartments have 2/3 BHK Configurations &amp; are Designed to Provide Ample Space &amp; Comfort. New Launch Project. Easy Payment Plan. Flexible Payment Plan. Budget Friendly.
-Pricing &amp; Floor Plan · Download Brochure · Runwal Group · Platinum Group · Adani Realty</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Locon Solutions Pvt. Ltd.</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Sponsored
-New Launch At Bhandup, Mumbai | New Launch At Bhandup
-lódháhomz.site
-https://www.lódháhomz.site › visit-site › enquire-now
-New Launch At Bhandup provides ultra-luxurious residences with the most breathtaking views
-E-Brochure · Pricing / Costing · Floor Plan · Project Overview</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>DIGITAL RUBIX</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -521,15 +520,15 @@
       <c r="A5" t="inlineStr">
         <is>
           <t>Sponsored
-Lodha Prelaunching Bhandup - 2 &amp; 3 BHK Starting ₹2.29 Cr*
-prelaunch-projects.in
-https://www.prelaunch-projects.in › lodhabhandup › luxuryhomes
-Get EOI and Early Bird Benefits, Prime location at LBS Road Bhandup by Lodha. Lodha...</t>
+New Launch At Bhandup - New Launch At Bhandup, Mumbai
+lódháhomz.site
+https://www.lódháhomz.site › site-visit › enquire-now
+Download Brochure — Its Big Apartments With 2/3 BHK, Its Prime Location Along The LBS...</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>PRELAUNCH REALTY PRIVATE LIMITED</t>
+          <t>DIGITAL RUBIX</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -542,58 +541,58 @@
       <c r="A6" t="inlineStr">
         <is>
           <t>Sponsored
-Lodha New Launch Bhandup | Luxury 2 &amp; 3 BHK
+Lodha® coming soon to LBS
+lodhagroup.in
+https://www.lodhagroup.in
+Lodha® LBS is Coming Soon — Live an exceptional lifestyle with forest living as Lodha comes to the prime LBS Marg. Lodha LBS along the Mulund-Bhandup-Kanjurmarg corridor ensures seamless connectivity.</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Macrotech Developers Limited</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Sponsored
+Lodha Prelaunching Bhandup | 2 &amp; 3 BHK Starting ₹2.29 Cr*
+prelaunch-projects.in
+https://www.prelaunch-projects.in
+Get EOI and Early Bird Benefits, Prime location at LBS Road Bhandup by Lodha. Lodha Bhandup 2 &amp; 3 BHK Homes Starting Price...
+Price Plans · Project Location · Site &amp; Floor Plan · Virtual Site Visit · The Amenities</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>PRELAUNCH REALTY PRIVATE LIMITED</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Sponsored
+Lodha New Launch Bhandup | 2/3 BHK Starts @ ₹ 2.29 Cr*
 bhandupnewlaunch.com
 https://www.bhandupnewlaunch.com › 2&amp;3bhk › luxury_homes
-Pre-book Lodha Bhandup at ₹1.08 Lacs* | Easy Access to Powai &amp; R-City Mall | EOI Open Now! Modern Living at Lodha Bhandup | 10 mins to Eastern Express Hwy | Pre-book at ₹1.08 Lacs* Free Pickup &amp; Drop. Avail Special Offers. Book Now.</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
+Free Pickup &amp; Drop — Pre-book Lodha Bhandup at ₹1.08 Lacs* | Easy Access to Powai &amp; R-City Mall | EOI Open Now! Modern Living at Lodha Bhandup | 10 mins to Eastern Express Hwy | Pre-book at ₹1.08 Lacs* Avail Special Offers.</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>Finwizz Holdings</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Sponsored
-Lodha® LBS is Coming Soon
-lodhagroup.in
-https://www.lodhagroup.in
-Lodha® coming soon to LBS — Live an exceptional lifestyle with forest living as Lodha comes to the prime LBS Marg. Lodha LBS along the Mulund-Bhandup-Kanjurmarg corridor ensures seamless connectivity.</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Macrotech Developers Limited</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Sponsored
-Lodha Bhandup | Lodha Bhandup New Launch
-propertymumbai.co.in
-http://www.propertymumbai.co.in › lodha_bhandup
-Book 2 &amp; 3 BHK Starts ₹2.29 Cr* &amp; Get EOI &amp; Early Bird Benefits at New Launch Bhandup West. its Big Apartments with 2/3 BHK, its prime Location along the LBS Road, Starts @ ₹ 2.29Cr* Download Brochure.
-Price · Floor Plan · Location · Amenities</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>NORA GROUP</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">

</xml_diff>

<commit_message>
UI for dashboard, Datatable
</commit_message>
<xml_diff>
--- a/scrapy/static/data/Lodha+bhandup+Ad+Advertiser.xlsx
+++ b/scrapy/static/data/Lodha+bhandup+Ad+Advertiser.xlsx
@@ -454,16 +454,16 @@
       <c r="A2" t="inlineStr">
         <is>
           <t>Sponsored
-Lodha Bhandup New Project - 2 &amp; 3 BHK @ ₹ 2.29 Cr All inc
-newproject-bhandup.co.in
-https://www.newproject-bhandup.co.in › lodha › new-launch
-Lodha New Launch Luxurious 2 &amp; 3 BHK apartments Starting Price from ₹ 2.29 Cr All Inc
-Price List · Brochure · Request Site Visit · Configuration</t>
+Lödha Bhandup West | Luxury 2, 2.5 &amp; 3 BHK
+l-bhandup.com
+https://www.l-bhandup.com › official
+Lödha on LBS Rd an upcoming residential project with the best of amenities ...
+Brochure &amp; Floor Plans · Price · View Project Highlights · Connect on Whatsapp</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>AddressofChoice Realty Pvt. Ltd</t>
+          <t>Rioga Premium Real Estate Advisory LLP</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -476,11 +476,11 @@
       <c r="A3" t="inlineStr">
         <is>
           <t>Sponsored
-Lodha Bhandup | New Project Launch in Bhandup
+Lodha New Launch Bhandup West | Download E-Brochure
 proptigermumbai.com
 https://www.proptigermumbai.com
-New Launch Project — its Big Apartments with 2/3 BHK, its prime Location along the LBS...
-Pricing &amp; Floor Plan · Download Brochure · Runwal Group · Platinum Group · Adani Realty</t>
+its Big Apartments with 2/3 BHK, its prime Location along the LBS Road, Starts @ ₹ 2.29Cr*
+Pricing &amp; Floor Plan · Download Brochure · Platinum Group · Transcon Developers</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -498,16 +498,16 @@
       <c r="A4" t="inlineStr">
         <is>
           <t>Sponsored
-Lödha Bhandup | Luxury 2, 2.5 &amp; 3 BHK | Avail Pre Launch Offer
-l-bhandup.com
-https://www.l-bhandup.com › official
-Excellent Connectivity — Lödha on LBS Rd an upcoming residential project with the best of...
-Brochure &amp; Floor Plans · Connect on Whatsapp · Price · View Project Highlights</t>
+New Launch At Bhandup
+lódháhomz.site
+https://www.lódháhomz.site › site-visit › enquire-now
+New Launch At Bhandup, Mumbai — Its Big Apartments With 2/3 BHK, Its Prime Location Along The LBS Road, Starts @ ₹ 2.29cr*
+E-Brochure · Floor Plan · Pricing / Costing · Project Overview</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Rioga Premium Real Estate Advisory LLP</t>
+          <t>DIGITAL RUBIX</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -520,15 +520,15 @@
       <c r="A5" t="inlineStr">
         <is>
           <t>Sponsored
-New Launch At Bhandup - New Launch At Bhandup, Mumbai
-lódháhomz.site
-https://www.lódháhomz.site › site-visit › enquire-now
-Download Brochure — Its Big Apartments With 2/3 BHK, Its Prime Location Along The LBS...</t>
+Lodha® LBS is Coming Soon | Near upcoming metro station
+lodhagroup.in
+https://www.lodhagroup.in
+Live an exceptional lifestyle with forest living as Lodha comes to the prime LBS Marg.</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>DIGITAL RUBIX</t>
+          <t>Macrotech Developers Limited</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -541,20 +541,22 @@
       <c r="A6" t="inlineStr">
         <is>
           <t>Sponsored
-Lodha® coming soon to LBS
-lodhagroup.in
-https://www.lodhagroup.in
-Lodha® LBS is Coming Soon — Live an exceptional lifestyle with forest living as Lodha comes to the prime LBS Marg. Lodha LBS along the Mulund-Bhandup-Kanjurmarg corridor ensures seamless connectivity.</t>
+Lodha Bhandup West Mumbai | 2&amp;3 BHK Apartment @ ₹2.29 CR*
+india-sales-office.com
+https://www.india-sales-office.com › official-site
+Starts at ₹2.29 CR* | The prime LBS Road, Mumbai | Modern Homes | Lots of Space &amp; Comfort. New launch project 2&amp;3 BHK luxury apartment by Lodha Group, location at Bhandup, Mumbai. Best Price Guaranteed.
+Floor Plans Details · View Price &amp; Payment Plan · Virtual Tour &amp; Video · Request Brochure
+Call us</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Macrotech Developers Limited</t>
+          <t>Property Junction International Real Estate Broker LLC</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>United Arab Emirates</t>
         </is>
       </c>
     </row>
@@ -562,16 +564,17 @@
       <c r="A7" t="inlineStr">
         <is>
           <t>Sponsored
-Lodha Prelaunching Bhandup | 2 &amp; 3 BHK Starting ₹2.29 Cr*
-prelaunch-projects.in
-https://www.prelaunch-projects.in
-Get EOI and Early Bird Benefits, Prime location at LBS Road Bhandup by Lodha. Lodha Bhandup 2 &amp; 3 BHK Homes Starting Price...
-Price Plans · Project Location · Site &amp; Floor Plan · Virtual Site Visit · The Amenities</t>
+Lodha Bhandup | Lodha in Bhandup West
+newlaunch-property.net
+https://www.newlaunch-property.net › lodha_bhandup
+Get Huge Discount On Booking. Schedule Your Free Site Visit &amp; Get Complete Project Details. Buy 2/3 BHK Premium Apartments by Lodha Property in Bhandup West, Mumbai @ ₹ 2.29 Cr*. Get Floor Plan. Download E Brochure.
+Floor Plans · Price List · Project Highlights
+Call us</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>PRELAUNCH REALTY PRIVATE LIMITED</t>
+          <t>GTF Technologies</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -584,15 +587,19 @@
       <c r="A8" t="inlineStr">
         <is>
           <t>Sponsored
-Lodha New Launch Bhandup | 2/3 BHK Starts @ ₹ 2.29 Cr*
-bhandupnewlaunch.com
-https://www.bhandupnewlaunch.com › 2&amp;3bhk › luxury_homes
-Free Pickup &amp; Drop — Pre-book Lodha Bhandup at ₹1.08 Lacs* | Easy Access to Powai &amp; R-City Mall | EOI Open Now! Modern Living at Lodha Bhandup | 10 mins to Eastern Express Hwy | Pre-book at ₹1.08 Lacs* Avail Special Offers.</t>
+Lodha Bhandup By Lodha group | 2 &amp; 3 BHK Homes at ₹ 2.29 Cr*
+newlaunch-bhandup.co.in
+https://www.newlaunch-bhandup.co.in › new_launch
+Established in 2012
+—
+Luxury 2 &amp; 3 BHK Homes Starts From ₹ 2.29 Cr* All Incl at Lodha Bhandup West, Mumbai. The project has easy access to both the Eastern Express Highway and the Eastern Motorway. Get The Best Rate.
+Site &amp; Floor Plans · Proposed Floor Plan · Pricing · Proposed Site Plan · View Gallery
+Call us</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Finwizz Holdings</t>
+          <t>Propertypistol Realty Pvt ltd</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">

</xml_diff>

<commit_message>
navbar UI for smaller screens, data table to dashboard routing
</commit_message>
<xml_diff>
--- a/scrapy/static/data/Lodha+bhandup+Ad+Advertiser.xlsx
+++ b/scrapy/static/data/Lodha+bhandup+Ad+Advertiser.xlsx
@@ -454,38 +454,40 @@
       <c r="A2" t="inlineStr">
         <is>
           <t>Sponsored
-Lödha Bhandup West | Luxury 2, 2.5 &amp; 3 BHK
+Lodha Bhandup New Project - 2 &amp; 3 BHK @ ₹ 2.29 Cr All Inc
+newproject-bhandup.co.in
+https://www.newproject-bhandup.co.in › lodha › new-launch
+Lodha LBS New Launch Luxurious 2 &amp; 3 BHK apartments Starting Price from ₹ 2.29 Cr All inc. Lodha Bhandup - Prelaunch Project...
+Price List
+Get Here Price List &amp; Floor Plan 2, 3 BHK Starts From ₹ 2.29 Cr
+Brochure
+Get Here Type, Size, Area &amp; Units Brochure Free</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>AddressofChoice Realty Pvt. Ltd</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Sponsored
+Lödha Bhandup | Luxury 2, 2.5 &amp; 3 BHK | Avail Pre Launch Offer
 l-bhandup.com
 https://www.l-bhandup.com › official
-Lödha on LBS Rd an upcoming residential project with the best of amenities ...
-Brochure &amp; Floor Plans · Price · View Project Highlights · Connect on Whatsapp</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
+Lödha on LBS Rd an upcoming residential project with the best of amenities &amp; views. Pre...</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>Rioga Premium Real Estate Advisory LLP</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Sponsored
-Lodha New Launch Bhandup West | Download E-Brochure
-proptigermumbai.com
-https://www.proptigermumbai.com
-its Big Apartments with 2/3 BHK, its prime Location along the LBS Road, Starts @ ₹ 2.29Cr*
-Pricing &amp; Floor Plan · Download Brochure · Platinum Group · Transcon Developers</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Locon Solutions Pvt. Ltd.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -498,11 +500,10 @@
       <c r="A4" t="inlineStr">
         <is>
           <t>Sponsored
-New Launch At Bhandup
+New Launch At Bhandup, Mumbai
 lódháhomz.site
 https://www.lódháhomz.site › site-visit › enquire-now
-New Launch At Bhandup, Mumbai — Its Big Apartments With 2/3 BHK, Its Prime Location Along The LBS Road, Starts @ ₹ 2.29cr*
-E-Brochure · Floor Plan · Pricing / Costing · Project Overview</t>
+New Launch At Bhandup — New Launch Project Presents 2 &amp; 3 BHK Apartments At Bhandup, Mumbai Starting At ₹ 2.29 Cr*</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -520,15 +521,15 @@
       <c r="A5" t="inlineStr">
         <is>
           <t>Sponsored
-Lodha® LBS is Coming Soon | Near upcoming metro station
-lodhagroup.in
-https://www.lodhagroup.in
-Live an exceptional lifestyle with forest living as Lodha comes to the prime LBS Marg.</t>
+Lodha Bhandup
+newlaunch-property.net
+https://www.newlaunch-property.net › lodha_bhandup
+Lodha in Bhandup West — Get Huge Discount On Booking. Schedule Your Free Site Visit &amp; Get Complete Project Details</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Macrotech Developers Limited</t>
+          <t>GTF Technologies</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -541,22 +542,21 @@
       <c r="A6" t="inlineStr">
         <is>
           <t>Sponsored
-Lodha Bhandup West Mumbai | 2&amp;3 BHK Apartment @ ₹2.29 CR*
-india-sales-office.com
-https://www.india-sales-office.com › official-site
-Starts at ₹2.29 CR* | The prime LBS Road, Mumbai | Modern Homes | Lots of Space &amp; Comfort. New launch project 2&amp;3 BHK luxury apartment by Lodha Group, location at Bhandup, Mumbai. Best Price Guaranteed.
-Floor Plans Details · View Price &amp; Payment Plan · Virtual Tour &amp; Video · Request Brochure
-Call us</t>
+Lodha Bhandup
+proptigermumbai.com
+https://www.proptigermumbai.com › lodha_newlaunch › bhandup_mumbai
+New Project Launch in Bhandup — its Big Apartments with 2/3 BHK, its prime Location along the LBS Road, Starts @ ₹ 2.29Cr* The Apartments have 2/3 BHK Configurations &amp; are Designed to Provide Ample Space &amp; Comfort. New Launch Project. Easy Payment Plan. Excellent Connectivity. Budget Friendly.
+Pricing &amp; Floor Plan · Download Brochure · Hiranandani Projects · Platinum Group</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Property Junction International Real Estate Broker LLC</t>
+          <t>Locon Solutions Pvt. Ltd.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>United Arab Emirates</t>
+          <t>India</t>
         </is>
       </c>
     </row>
@@ -564,17 +564,15 @@
       <c r="A7" t="inlineStr">
         <is>
           <t>Sponsored
-Lodha Bhandup | Lodha in Bhandup West
-newlaunch-property.net
-https://www.newlaunch-property.net › lodha_bhandup
-Get Huge Discount On Booking. Schedule Your Free Site Visit &amp; Get Complete Project Details. Buy 2/3 BHK Premium Apartments by Lodha Property in Bhandup West, Mumbai @ ₹ 2.29 Cr*. Get Floor Plan. Download E Brochure.
-Floor Plans · Price List · Project Highlights
-Call us</t>
+Lodha Bhandup New Launch | 2/3 BHK Starts @ ₹ 2.29 Cr*
+bhandupnewlaunch.com
+https://www.bhandupnewlaunch.com › 2&amp;3bhk › luxury_homes
+Pre-book Lodha Bhandup at ₹1.08 Lacs* | Easy Access to Powai &amp; R-City Mall | EOI Open Now! Modern Living at Lodha Bhandup | 10 mins to Eastern Express Hwy | Pre-book at ₹1.08 Lacs* Free Pickup &amp; Drop.</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>GTF Technologies</t>
+          <t>Finwizz Holdings</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -587,19 +585,16 @@
       <c r="A8" t="inlineStr">
         <is>
           <t>Sponsored
-Lodha Bhandup By Lodha group | 2 &amp; 3 BHK Homes at ₹ 2.29 Cr*
-newlaunch-bhandup.co.in
-https://www.newlaunch-bhandup.co.in › new_launch
-Established in 2012
-—
-Luxury 2 &amp; 3 BHK Homes Starts From ₹ 2.29 Cr* All Incl at Lodha Bhandup West, Mumbai. The project has easy access to both the Eastern Express Highway and the Eastern Motorway. Get The Best Rate.
-Site &amp; Floor Plans · Proposed Floor Plan · Pricing · Proposed Site Plan · View Gallery
-Call us</t>
+Lodha Bhandup | Lodha New Launch Bhandup
+preferred-partners.co.in
+http://www.preferred-partners.co.in › lodha_bhandup › book_now
+Lodha Bhandup Premium 2 &amp; 3 BHK Homes Starts ₹ 2.29 Cr* On Request at Bhandup West, Mumbai. The Apartments have 2/3 BHK Configurations &amp; are Designed to Provide Ample Space &amp; Comfort. Limited Deals Available.
+Download Brochure · Pricing /Costing · Book a Site Visit · Top Facilities</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Propertypistol Realty Pvt ltd</t>
+          <t>INVESTOXPERT ADVISORS PRIVATE LIMITED</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">

</xml_diff>